<commit_message>
Add simple password authentication to the application. Now users can sign up with a password. The server only allows an account to have one session signed into it.
</commit_message>
<xml_diff>
--- a/etc/2171-SWEN-261-b-Bethesda.xlsx
+++ b/etc/2171-SWEN-261-b-Bethesda.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="84">
   <si>
     <t>Instructions</t>
   </si>
@@ -209,9 +209,6 @@
   </si>
   <si>
     <t>Name</t>
-  </si>
-  <si>
-    <t>JONNNIE YOURE A BITCH</t>
   </si>
   <si>
     <t>As a player I want to convert my standard pieces into king pieces whenever they reach the opponent's side of the board so that my pieces have more possible moves.</t>
@@ -989,10 +986,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AMK49"/>
   <sheetViews>
-    <sheetView windowProtection="1" tabSelected="1" topLeftCell="A36" zoomScale="65" zoomScaleNormal="65" workbookViewId="0">
+    <sheetView windowProtection="1" tabSelected="1" topLeftCell="A14" zoomScale="65" zoomScaleNormal="65" workbookViewId="0">
       <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
       <selection activeCell="A13" sqref="A13"/>
-      <selection pane="topRight" activeCell="B46" sqref="B46"/>
+      <selection pane="topRight" activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -1318,9 +1315,6 @@
         <v>36</v>
       </c>
       <c r="C19" s="8"/>
-      <c r="D19" s="3" t="s">
-        <v>59</v>
-      </c>
       <c r="E19" s="8"/>
       <c r="F19" s="15"/>
       <c r="G19" s="8"/>
@@ -1409,139 +1403,139 @@
     </row>
     <row r="32" spans="1:8" ht="94.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A32" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="B32" s="18" t="s">
         <v>60</v>
-      </c>
-      <c r="B32" s="18" t="s">
-        <v>61</v>
       </c>
       <c r="C32" s="23"/>
       <c r="D32" s="18"/>
     </row>
     <row r="33" spans="1:4" ht="125.4" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A33" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="B33" s="3" t="s">
         <v>62</v>
-      </c>
-      <c r="B33" s="3" t="s">
-        <v>63</v>
       </c>
       <c r="C33" s="24"/>
     </row>
     <row r="34" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
       <c r="B34" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C34" s="24"/>
     </row>
     <row r="35" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A35" s="18"/>
       <c r="B35" s="18" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C35" s="23"/>
       <c r="D35" s="18"/>
     </row>
     <row r="36" spans="1:4" ht="63" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A36" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="B36" s="3" t="s">
         <v>66</v>
-      </c>
-      <c r="B36" s="3" t="s">
-        <v>67</v>
       </c>
       <c r="C36" s="24"/>
     </row>
     <row r="37" spans="1:4" ht="62.4" x14ac:dyDescent="0.3">
       <c r="A37" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="B37" s="3" t="s">
         <v>68</v>
-      </c>
-      <c r="B37" s="3" t="s">
-        <v>69</v>
       </c>
       <c r="C37" s="24"/>
     </row>
     <row r="38" spans="1:4" ht="47.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A38" s="18"/>
       <c r="B38" s="18" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C38" s="23"/>
       <c r="D38" s="18"/>
     </row>
     <row r="39" spans="1:4" ht="78.599999999999994" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A39" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="B39" s="3" t="s">
         <v>71</v>
-      </c>
-      <c r="B39" s="3" t="s">
-        <v>72</v>
       </c>
       <c r="C39" s="24"/>
     </row>
     <row r="40" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
       <c r="B40" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C40" s="24"/>
     </row>
     <row r="41" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
       <c r="B41" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C41" s="24"/>
     </row>
     <row r="42" spans="1:4" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A42" s="18"/>
       <c r="B42" s="18" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C42" s="23"/>
       <c r="D42" s="18"/>
     </row>
     <row r="43" spans="1:4" ht="109.8" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A43" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="B43" s="3" t="s">
         <v>76</v>
-      </c>
-      <c r="B43" s="3" t="s">
-        <v>77</v>
       </c>
       <c r="C43" s="24"/>
     </row>
     <row r="44" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
       <c r="B44" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C44" s="24"/>
     </row>
     <row r="45" spans="1:4" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A45" s="18"/>
       <c r="B45" s="18" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C45" s="23"/>
       <c r="D45" s="18"/>
     </row>
     <row r="46" spans="1:4" ht="47.4" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A46" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="B46" s="3" t="s">
         <v>80</v>
-      </c>
-      <c r="B46" s="3" t="s">
-        <v>81</v>
       </c>
       <c r="C46" s="24"/>
     </row>
     <row r="47" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
       <c r="B47" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C47" s="24"/>
     </row>
     <row r="48" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
       <c r="B48" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C48" s="24"/>
     </row>
     <row r="49" spans="2:3" ht="46.8" x14ac:dyDescent="0.3">
       <c r="B49" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C49" s="24"/>
     </row>
@@ -1594,7 +1588,7 @@
       <formula>AND(ISBLANK(D17),C17="Fail")</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations disablePrompts="1" count="1">
+  <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C19 E2:E19 G2:G19" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>"Pass,Fail"</formula1>
       <formula2>0</formula2>

</xml_diff>